<commit_message>
date? o no date? the looong way
</commit_message>
<xml_diff>
--- a/TestCasesTemplate.xlsx
+++ b/TestCasesTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless_69du903\OneDrive\Documents\Escuela\Universidad UPAEP\Sexto Semestre\Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless_69du903\OneDrive\Documents\Programming\GITHUB\Sistema-de-Citas-Pasaporte-PruebasSFW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8351FFEE-1A4F-46E3-9973-5ED71BC75288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC05826A-B224-4569-9C6D-651FC2A4C408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{11E442AE-7DC1-4263-8F6A-AE63186D4D47}"/>
   </bookViews>

</xml_diff>